<commit_message>
added empty step definitions for skill and user controller
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -110,7 +110,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_Jan10"
+"skillName": "Team1_SeleniummUpdated"
 }</t>
   </si>
   <si>
@@ -123,13 +123,26 @@
     <t>CreateSkill_Valid_MissingValues</t>
   </si>
   <si>
+    <t>{
+}</t>
+  </si>
+  <si>
     <t>GetALL_SkillMaster</t>
+  </si>
+  <si>
+    <t>/allSkillMaster</t>
   </si>
   <si>
     <t>GetSkill_Valid</t>
   </si>
   <si>
+    <t>/skills/{skillMasterName}</t>
+  </si>
+  <si>
     <t>GetSkill_InValid</t>
+  </si>
+  <si>
+    <t>/skills/invalid10000</t>
   </si>
   <si>
     <t>UpdateSkill_Valid</t>
@@ -148,7 +161,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -190,6 +203,11 @@
       <name val="Times New Roman"/>
     </font>
     <font>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="12.0"/>
       <color rgb="FF181818"/>
       <name val="Times New Roman"/>
@@ -215,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -243,7 +261,10 @@
     <xf borderId="0" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="7" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="8" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
   </cellXfs>
@@ -6672,7 +6693,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="33.13"/>
-    <col customWidth="1" min="2" max="2" width="26.13"/>
+    <col customWidth="1" min="2" max="2" width="28.63"/>
     <col customWidth="1" min="3" max="3" width="13.63"/>
     <col customWidth="1" min="4" max="4" width="17.63"/>
     <col customWidth="1" min="5" max="5" width="72.88"/>
@@ -6697,7 +6718,7 @@
       <c r="A2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="9" t="s">
         <v>27</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -6711,55 +6732,91 @@
       <c r="A3" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="9"/>
+      <c r="B3" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" s="3">
+        <v>400.0</v>
+      </c>
+      <c r="E3" s="10"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="9"/>
+      <c r="B4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="3">
+        <v>500.0</v>
+      </c>
+      <c r="E4" s="10"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
-      <c r="E5" s="9"/>
+      <c r="C5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="3">
+        <v>200.0</v>
+      </c>
+      <c r="E5" s="10"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
-      <c r="E6" s="9"/>
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3">
+        <v>200.0</v>
+      </c>
+      <c r="E6" s="10"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
-      <c r="E7" s="9"/>
+      <c r="C7" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="3">
+        <v>404.0</v>
+      </c>
+      <c r="E7" s="10"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
-      <c r="E8" s="9"/>
+      <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
-      <c r="E9" s="9"/>
+      <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
-      <c r="E10" s="9"/>
+      <c r="E10" s="10"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
-      <c r="E11" s="9"/>
+      <c r="E11" s="10"/>
     </row>
     <row r="12" ht="15.75" customHeight="1"/>
     <row r="13" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
completed post and get scenarios in skill module
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -13,14 +13,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="C3Qx8ow7TWDhbqIalr3xZ7AZDR1tChjYGEDA2UHbuaM="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="2S3C65u/rDy8qjmzty8FRCCttiD7UJteggYR8WMafpU="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -34,19 +34,55 @@
     <t>ExpectedStatusCode</t>
   </si>
   <si>
-    <t>CreateBatch_Valid_batchName</t>
+    <t>CreateBatch_Valid_Request</t>
   </si>
   <si>
     <t>{
-"batchDescription": "Test batch",
-"batchName": "SDETTeam1",
+"batchDescription": "",
+"batchName": "",
 "batchNoOfClasses": 1,
 "batchStatus": "Active",
-"programId": 13
+"programId": 3
 }</t>
   </si>
   <si>
     <t>/batches</t>
+  </si>
+  <si>
+    <t>CreateBatch_NoAuth</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "Test",
+"batchName": "TestBatch1",
+"batchNoOfClasses": 1,
+"batchStatus": "Active",
+"programId": 3
+}</t>
+  </si>
+  <si>
+    <t>CreateBatch_Existing_Batch</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "Test",
+"batchName": "Batch1",
+"batchNoOfClasses": 1,
+"batchStatus": "Active",
+"programId": 3
+}</t>
+  </si>
+  <si>
+    <t>CreateBatch_Missing_Fields</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "Test",
+"batchName": "Batch1",
+"batchNoOfClasses": ,
+"batchStatus": "Active",
+"programId": 3
+}</t>
   </si>
   <si>
     <t>CreateAdmin_valid_newValues</t>
@@ -110,7 +146,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_SeleniummUpdated"
+"skillName": "Team1_PlaywrightUpdated"
 }</t>
   </si>
   <si>
@@ -154,7 +190,13 @@
     <t>DeleteSkill_Valid</t>
   </si>
   <si>
+    <t>/deletebySkillId/{skillId}</t>
+  </si>
+  <si>
     <t>DeleteSkill_InValid</t>
+  </si>
+  <si>
+    <t>/deletebySkillId/10000000</t>
   </si>
 </sst>
 </file>
@@ -2536,7 +2578,7 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="30.25"/>
+    <col customWidth="1" min="1" max="1" width="37.75"/>
     <col customWidth="1" min="2" max="2" width="47.38"/>
     <col customWidth="1" min="3" max="3" width="17.75"/>
     <col customWidth="1" min="4" max="4" width="21.5"/>
@@ -2571,9 +2613,48 @@
         <v>201.0</v>
       </c>
     </row>
-    <row r="3" ht="15.75" customHeight="1"/>
-    <row r="4" ht="15.75" customHeight="1"/>
-    <row r="5" ht="15.75" customHeight="1"/>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="4">
+        <v>401.0</v>
+      </c>
+    </row>
+    <row r="4" ht="15.75" customHeight="1">
+      <c r="A4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="4">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="5" ht="15.75" customHeight="1">
+      <c r="A5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="4">
+        <v>400.0</v>
+      </c>
+    </row>
     <row r="6" ht="15.75" customHeight="1"/>
     <row r="7" ht="15.75" customHeight="1"/>
     <row r="8" ht="15.75" customHeight="1"/>
@@ -3568,7 +3649,6 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
-    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3608,124 +3688,124 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>17</v>
+        <v>23</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>21</v>
+        <v>27</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>22</v>
+        <v>28</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="G20" s="7"/>
     </row>
@@ -6716,13 +6796,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>26</v>
+        <v>32</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D2" s="3">
         <v>201.0</v>
@@ -6730,13 +6810,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>27</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D3" s="3">
         <v>400.0</v>
@@ -6745,13 +6825,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="D4" s="3">
         <v>500.0</v>
@@ -6760,10 +6840,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="D5" s="3">
         <v>200.0</v>
@@ -6772,10 +6852,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="D6" s="3">
         <v>200.0</v>
@@ -6784,10 +6864,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="D7" s="3">
         <v>404.0</v>
@@ -6796,25 +6876,37 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="3">
+        <v>200.0</v>
       </c>
       <c r="E10" s="10"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>41</v>
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D11" s="3">
+        <v>404.0</v>
       </c>
       <c r="E11" s="10"/>
     </row>

</xml_diff>

<commit_message>
completed skill master scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -13,14 +13,14 @@
   <calcPr/>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion2">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="2S3C65u/rDy8qjmzty8FRCCttiD7UJteggYR8WMafpU="/>
+      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId9" roundtripDataChecksum="C3Qx8ow7TWDhbqIalr3xZ7AZDR1tChjYGEDA2UHbuaM="/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="61">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -73,7 +73,7 @@
 }</t>
   </si>
   <si>
-    <t>CreateBatch_Missing_Fields</t>
+    <t>CreateBatch_Missing_Mandatory_Fields</t>
   </si>
   <si>
     <t>{
@@ -82,6 +82,48 @@
 "batchNoOfClasses": ,
 "batchStatus": "Active",
 "programId": 3
+}</t>
+  </si>
+  <si>
+    <t>CreateBatch_invalid_endpoint</t>
+  </si>
+  <si>
+    <t>/batch</t>
+  </si>
+  <si>
+    <t>CreateBatch_Missing_Additional_Fields</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "",
+"batchName": "TestBatch1",
+"batchNoOfClasses": 1,
+"batchStatus": "Active",
+"programId": 3
+}</t>
+  </si>
+  <si>
+    <t>CreateBatch_invalid_data</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "Test",
+"Name": "TestBatch1",
+"batchNoOfClasses": 1,
+"batchStatus": "Active",
+"programId": 47
+}</t>
+  </si>
+  <si>
+    <t>CreateBatch_inactive_programId</t>
+  </si>
+  <si>
+    <t>{
+"batchDescription": "Test",
+"batchName": "TestBatch1",
+"batchNoOfClasses": 1,
+"batchStatus": "Active",
+"programId": 47
 }</t>
   </si>
   <si>
@@ -146,7 +188,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_PlaywrightUpdated"
+"skillName": "Team1_Cypress"
 }</t>
   </si>
   <si>
@@ -184,7 +226,18 @@
     <t>UpdateSkill_Valid</t>
   </si>
   <si>
+    <t>{
+"skillName": "Team1_CypressUpdated"
+}</t>
+  </si>
+  <si>
+    <t>/updateSkills/{skillId}</t>
+  </si>
+  <si>
     <t>UpdateSkill_InValid</t>
+  </si>
+  <si>
+    <t>/updateSkills/100000</t>
   </si>
   <si>
     <t>DeleteSkill_Valid</t>
@@ -2655,10 +2708,62 @@
         <v>400.0</v>
       </c>
     </row>
-    <row r="6" ht="15.75" customHeight="1"/>
-    <row r="7" ht="15.75" customHeight="1"/>
-    <row r="8" ht="15.75" customHeight="1"/>
-    <row r="9" ht="15.75" customHeight="1"/>
+    <row r="6" ht="15.75" customHeight="1">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="4">
+        <v>404.0</v>
+      </c>
+    </row>
+    <row r="7" ht="15.75" customHeight="1">
+      <c r="A7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4">
+        <v>201.0</v>
+      </c>
+    </row>
+    <row r="8" ht="15.75" customHeight="1">
+      <c r="A8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8" s="4">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="9" ht="15.75" customHeight="1">
+      <c r="A9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9" s="4">
+        <v>400.0</v>
+      </c>
+    </row>
     <row r="10" ht="15.75" customHeight="1"/>
     <row r="11" ht="15.75" customHeight="1"/>
     <row r="12" ht="15.75" customHeight="1"/>
@@ -3649,6 +3754,7 @@
     <row r="997" ht="15.75" customHeight="1"/>
     <row r="998" ht="15.75" customHeight="1"/>
     <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3688,124 +3794,124 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="F2" s="6"/>
       <c r="G2" s="7"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="G3" s="7"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="G4" s="7"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="F5" s="6"/>
       <c r="G5" s="7"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="F6" s="6"/>
       <c r="G6" s="7"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="G7" s="7"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="F8" s="6"/>
       <c r="G8" s="7"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="F9" s="6"/>
       <c r="G9" s="7"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F10" s="6"/>
       <c r="G10" s="7"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="G11" s="7"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="G12" s="7"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F13" s="8"/>
       <c r="G13" s="7"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G14" s="7"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="G15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="F16" s="6"/>
       <c r="G16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="G17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="3" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
       <c r="G18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="3" t="s">
-        <v>30</v>
+        <v>38</v>
       </c>
       <c r="F19" s="6"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="3" t="s">
-        <v>31</v>
+        <v>39</v>
       </c>
       <c r="G20" s="7"/>
     </row>
@@ -6774,7 +6880,7 @@
   <cols>
     <col customWidth="1" min="1" max="1" width="33.13"/>
     <col customWidth="1" min="2" max="2" width="28.63"/>
-    <col customWidth="1" min="3" max="3" width="13.63"/>
+    <col customWidth="1" min="3" max="3" width="21.75"/>
     <col customWidth="1" min="4" max="4" width="17.63"/>
     <col customWidth="1" min="5" max="5" width="72.88"/>
     <col customWidth="1" min="6" max="6" width="12.63"/>
@@ -6796,13 +6902,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="3" t="s">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D2" s="3">
         <v>201.0</v>
@@ -6810,13 +6916,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3">
         <v>400.0</v>
@@ -6825,13 +6931,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>36</v>
+        <v>44</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>34</v>
+        <v>42</v>
       </c>
       <c r="D4" s="3">
         <v>500.0</v>
@@ -6840,10 +6946,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="3" t="s">
-        <v>38</v>
+        <v>46</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>39</v>
+        <v>47</v>
       </c>
       <c r="D5" s="3">
         <v>200.0</v>
@@ -6852,10 +6958,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3">
         <v>200.0</v>
@@ -6864,10 +6970,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>43</v>
+        <v>51</v>
       </c>
       <c r="D7" s="3">
         <v>404.0</v>
@@ -6876,22 +6982,40 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>44</v>
+        <v>52</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D8" s="3">
+        <v>200.0</v>
       </c>
       <c r="E8" s="10"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>45</v>
+        <v>55</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D9" s="3">
+        <v>400.0</v>
       </c>
       <c r="E9" s="10"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>46</v>
+        <v>57</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>47</v>
+        <v>58</v>
       </c>
       <c r="D10" s="3">
         <v>200.0</v>
@@ -6900,10 +7024,10 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>49</v>
+        <v>60</v>
       </c>
       <c r="D11" s="3">
         <v>404.0</v>

</xml_diff>

<commit_message>
implemented api chaining for skill master and user controller
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="458" uniqueCount="310">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="333">
   <si>
     <t>ScenarioName</t>
   </si>
@@ -457,6 +457,12 @@
   <si>
     <t xml:space="preserve">      |CreateProgram_with_Valid_ProgramDesc_ProgramName_Active_Status    |
 </t>
+  </si>
+  <si>
+    <t>GetProgramById_with_Invalid_Endpoint</t>
+  </si>
+  <si>
+    <t>/programs/{programId}</t>
   </si>
   <si>
     <t>Comments</t>
@@ -642,6 +648,84 @@
     <t>/batches/programs/{programId}</t>
   </si>
   <si>
+    <t>PutBatchById_Valid_BatchId</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+"batchDescription": "test", 
+"batchId": 0, 
+"batchName": "", 
+"batchNoOfClasses": 1, 
+"batchStatus": "Active", 
+"programId": "", 
+"programName": "" 
+}
+</t>
+  </si>
+  <si>
+    <t>/batches/{batchId}</t>
+  </si>
+  <si>
+    <t>PutBatchById_Invalid_BatchId</t>
+  </si>
+  <si>
+    <t>PutBatchById_NoAuth</t>
+  </si>
+  <si>
+    <t>PutBatchById_Invalid_Endpoint</t>
+  </si>
+  <si>
+    <t>/batch/{batchId}</t>
+  </si>
+  <si>
+    <t>PutBatchById_Missing_Mandatory_Fields</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+"batchDescription": "test", 
+"batchId": 0, 
+"batchName": "", 
+"batchStatus": "Active", 
+"programId": "", 
+"programName": "" 
+}
+</t>
+  </si>
+  <si>
+    <t>PutBatchById_Missing_Additional_Fields</t>
+  </si>
+  <si>
+    <t>{ 
+"batchId": 0, 
+"batchName": "", 
+"batchNoOfClasses": 1, 
+"batchStatus": "Active", 
+"programId": "", 
+"programName": "" 
+}</t>
+  </si>
+  <si>
+    <t>PutBatchById_Invalid_Data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{ 
+"batchDescription": "test",
+"batchId": 0, 
+"batchName": "",
+"batchNoOfClasses": "ten", 
+"batchStatus": "Active", 
+"programId": "", 
+"programName": "" 
+}
+</t>
+  </si>
+  <si>
+    <t>PutBatchById_Deleted_programId</t>
+  </si>
+  <si>
+    <t>PutBatchById_Deleted_BatchId</t>
+  </si>
+  <si>
     <t>ExpectedStatusMessage</t>
   </si>
   <si>
@@ -665,7 +749,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teaaapi13@gmail.co</t>
+      <t>teaaapi14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -683,7 +767,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6232323209</t>
+      <t>+1 7232323209</t>
     </r>
     <r>
       <rPr>
@@ -730,7 +814,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapi13@gmail.co</t>
+      <t>teamapi14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -773,7 +857,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapia13@gmail.co</t>
+      <t>teamapia14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -791,7 +875,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6000110009</t>
+      <t>+1 7000110009</t>
     </r>
     <r>
       <rPr>
@@ -836,7 +920,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiab13@gmail.co</t>
+      <t>teamapiab14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -854,7 +938,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6000111009</t>
+      <t>+1 7000111009</t>
     </r>
     <r>
       <rPr>
@@ -899,7 +983,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabc13@gmail.co</t>
+      <t>teamapiabc14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -917,7 +1001,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6001111009</t>
+      <t>+1 7001111009</t>
     </r>
     <r>
       <rPr>
@@ -962,7 +1046,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcd13@gmail.co</t>
+      <t>teamapiabcd14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -980,7 +1064,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6011111009</t>
+      <t>+1 7011111009</t>
     </r>
     <r>
       <rPr>
@@ -1025,7 +1109,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabce13@gmail.co</t>
+      <t>teamapiabce14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1043,7 +1127,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6111111009</t>
+      <t>+1 7111111009</t>
     </r>
     <r>
       <rPr>
@@ -1088,7 +1172,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcf13@gmail.co</t>
+      <t>teamapiabcf14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1106,7 +1190,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6211111009</t>
+      <t>+1 7211111009</t>
     </r>
     <r>
       <rPr>
@@ -1151,7 +1235,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcg13@gmail.co</t>
+      <t>teamapiabcg14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1169,7 +1253,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6221111009</t>
+      <t>+1 7221111009</t>
     </r>
     <r>
       <rPr>
@@ -1214,7 +1298,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabch13@gmail.co</t>
+      <t>teamapiabch14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1232,7 +1316,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6222111009</t>
+      <t>+1 7222111009</t>
     </r>
     <r>
       <rPr>
@@ -1277,7 +1361,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabci13@gmail.co</t>
+      <t>teamapiabci14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1295,7 +1379,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6222211009</t>
+      <t>+1 7222211009</t>
     </r>
     <r>
       <rPr>
@@ -1340,7 +1424,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcj13@gmail.co</t>
+      <t>teamapiabcj14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1358,7 +1442,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6222221009</t>
+      <t>+1 7222221009</t>
     </r>
     <r>
       <rPr>
@@ -1403,7 +1487,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabck13@gmail.co</t>
+      <t>teamapiabck14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1421,7 +1505,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6222222009</t>
+      <t>+1 7222222009</t>
     </r>
     <r>
       <rPr>
@@ -1466,7 +1550,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcl13@gmail.co</t>
+      <t>teamapiabcl14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1484,7 +1568,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6222222209</t>
+      <t>+1 7222222209</t>
     </r>
     <r>
       <rPr>
@@ -1529,7 +1613,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcm13@gmail.co</t>
+      <t>teamapiabcm14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1547,7 +1631,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6322222209</t>
+      <t>+1 7322222209</t>
     </r>
     <r>
       <rPr>
@@ -1592,7 +1676,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcn13@gmail.co</t>
+      <t>teamapiabcn14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1610,7 +1694,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6332222209</t>
+      <t>+1 7332222209</t>
     </r>
     <r>
       <rPr>
@@ -1655,7 +1739,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabco13@gmail.co</t>
+      <t>teamapiabco14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1673,7 +1757,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6333222209</t>
+      <t>+1 7333222209</t>
     </r>
     <r>
       <rPr>
@@ -1718,7 +1802,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcp13@gmail.co</t>
+      <t>teamapiabcp14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1736,7 +1820,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6333322209</t>
+      <t>+1 7333322209</t>
     </r>
     <r>
       <rPr>
@@ -1781,7 +1865,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcq13@gmail.co</t>
+      <t>teamapiabcq14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1799,7 +1883,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6333332209</t>
+      <t>+1 7333332209</t>
     </r>
     <r>
       <rPr>
@@ -1844,7 +1928,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcr13@gmail.co</t>
+      <t>teamapiabcr14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1862,7 +1946,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6433332209</t>
+      <t>+1 7433332209</t>
     </r>
     <r>
       <rPr>
@@ -1907,7 +1991,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcs13@gmail.co</t>
+      <t>teamapiabcs14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1960,7 +2044,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2008,7 +2092,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2059,7 +2143,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2110,7 +2194,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2162,7 +2246,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2213,7 +2297,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2264,7 +2348,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2315,7 +2399,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2361,7 +2445,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6443332209</t>
+      <t>+1 7443332209</t>
     </r>
     <r>
       <rPr>
@@ -2409,7 +2493,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabct13@gmail.co</t>
+      <t>teamapiabct14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2427,7 +2511,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6444332209</t>
+      <t>+1 7444332209</t>
     </r>
     <r>
       <rPr>
@@ -2471,7 +2555,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcu13@gmail.co</t>
+      <t>teamapiabcu14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2489,7 +2573,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6444432209</t>
+      <t>+1 7444432209</t>
     </r>
     <r>
       <rPr>
@@ -2533,7 +2617,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcv13@gmail.co</t>
+      <t>teamapiabcv14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2551,7 +2635,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6544332209</t>
+      <t>+1 7544332209</t>
     </r>
     <r>
       <rPr>
@@ -2595,7 +2679,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcw13@gmail.co</t>
+      <t>teamapiabcw14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2613,7 +2697,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6554332209</t>
+      <t>+1 7554332209</t>
     </r>
     <r>
       <rPr>
@@ -2657,7 +2741,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcx13@gmail.co</t>
+      <t>teamapiabcx14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2675,7 +2759,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 6555332209</t>
+      <t>+1 7555332209</t>
     </r>
     <r>
       <rPr>
@@ -2719,7 +2803,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcy13@gmail.co</t>
+      <t>teamapiabcy14@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2837,10 +2921,28 @@
     <t>/users/programs/{programId}</t>
   </si>
   <si>
-    <t>Gets Users by roleId</t>
+    <t>Gets_Users_by_roleId</t>
   </si>
   <si>
     <t>/users/roles/{roleId}</t>
+  </si>
+  <si>
+    <t>Gets_Users_by_roleId_v2</t>
+  </si>
+  <si>
+    <t>/v2/users</t>
+  </si>
+  <si>
+    <t>Get_Batch_by_UserId</t>
+  </si>
+  <si>
+    <t>/users/user/{userId}</t>
+  </si>
+  <si>
+    <t>Get_User_Details_by_Id</t>
+  </si>
+  <si>
+    <t>/users/details/{id}</t>
   </si>
   <si>
     <t>DeleteAdmin_validUser</t>
@@ -3029,9 +3131,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12.0"/>
-      <color rgb="FF000000"/>
-      <name val="&quot;Menlo&quot;"/>
+      <sz val="11.0"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <b/>
@@ -3158,8 +3260,8 @@
     <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="3" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="3" fontId="13" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
@@ -4926,8 +5028,9 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="68.38"/>
-    <col customWidth="1" min="2" max="2" width="100.25"/>
-    <col customWidth="1" min="3" max="4" width="12.63"/>
+    <col customWidth="1" min="2" max="2" width="57.88"/>
+    <col customWidth="1" min="3" max="3" width="19.25"/>
+    <col customWidth="1" min="4" max="4" width="12.63"/>
     <col customWidth="1" min="5" max="5" width="21.0"/>
     <col customWidth="1" min="6" max="6" width="18.88"/>
   </cols>
@@ -5224,7 +5327,23 @@
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1"/>
-    <row r="17" ht="15.75" customHeight="1"/>
+    <row r="17" ht="15.75" customHeight="1">
+      <c r="A17" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>113</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="13">
+        <v>404.0</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="18" ht="15.75" customHeight="1"/>
     <row r="19" ht="15.75" customHeight="1"/>
     <row r="20" ht="15.75" customHeight="1"/>
@@ -6248,18 +6367,18 @@
         <v>78</v>
       </c>
       <c r="F1" s="13" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="15" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D2" s="16">
         <v>201.0</v>
@@ -6267,13 +6386,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="15" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="C3" s="13" t="s">
         <v>117</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>115</v>
       </c>
       <c r="D3" s="16">
         <v>401.0</v>
@@ -6281,47 +6400,47 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="15" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D4" s="16">
         <v>400.0</v>
       </c>
       <c r="E4" s="13" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="15" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D5" s="16">
         <v>400.0</v>
       </c>
       <c r="E5" s="17" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="15" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D6" s="16">
         <v>404.0</v>
@@ -6329,64 +6448,64 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="15" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D7" s="16">
         <v>201.0</v>
       </c>
       <c r="F7" s="13" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="15" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D8" s="16">
         <v>400.0</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="15" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D9" s="16">
         <v>400.0</v>
       </c>
       <c r="E9" s="17" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D10" s="16">
         <v>200.0</v>
@@ -6394,10 +6513,10 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="D11" s="16">
         <v>401.0</v>
@@ -6405,10 +6524,10 @@
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="13" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="D12" s="16">
         <v>404.0</v>
@@ -6416,10 +6535,10 @@
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D13" s="16">
         <v>200.0</v>
@@ -6427,10 +6546,10 @@
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="D14" s="16">
         <v>401.0</v>
@@ -6438,24 +6557,24 @@
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="13" t="s">
+        <v>144</v>
+      </c>
+      <c r="C15" s="13" t="s">
         <v>142</v>
-      </c>
-      <c r="C15" s="13" t="s">
-        <v>140</v>
       </c>
       <c r="D15" s="16">
         <v>404.0</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="D16" s="16">
         <v>404.0</v>
@@ -6463,24 +6582,24 @@
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="13" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D17" s="16">
         <v>200.0</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="C18" s="13" t="s">
         <v>149</v>
-      </c>
-      <c r="C18" s="13" t="s">
-        <v>147</v>
       </c>
       <c r="D18" s="16">
         <v>401.0</v>
@@ -6488,10 +6607,10 @@
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="13" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="D19" s="16">
         <v>404.0</v>
@@ -6502,10 +6621,10 @@
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="13" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="D20" s="16">
         <v>404.0</v>
@@ -6513,10 +6632,10 @@
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="13" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D21" s="16">
         <v>200.0</v>
@@ -6524,10 +6643,10 @@
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="D22" s="16">
         <v>404.0</v>
@@ -6538,10 +6657,10 @@
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="13" t="s">
+        <v>158</v>
+      </c>
+      <c r="C23" s="13" t="s">
         <v>156</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>154</v>
       </c>
       <c r="D23" s="16">
         <v>401.0</v>
@@ -6549,24 +6668,141 @@
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="13" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="D24" s="16">
         <v>404.0</v>
       </c>
     </row>
-    <row r="25" ht="15.75" customHeight="1"/>
-    <row r="26" ht="15.75" customHeight="1"/>
-    <row r="27" ht="15.75" customHeight="1"/>
-    <row r="28" ht="15.75" customHeight="1"/>
-    <row r="29" ht="15.75" customHeight="1"/>
-    <row r="30" ht="15.75" customHeight="1"/>
-    <row r="31" ht="15.75" customHeight="1"/>
-    <row r="32" ht="15.75" customHeight="1"/>
-    <row r="33" ht="15.75" customHeight="1"/>
+    <row r="25" ht="15.75" customHeight="1">
+      <c r="A25" s="13" t="s">
+        <v>161</v>
+      </c>
+      <c r="B25" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D25" s="13">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="26" ht="15.75" customHeight="1">
+      <c r="A26" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D26" s="13">
+        <v>404.0</v>
+      </c>
+    </row>
+    <row r="27" ht="15.75" customHeight="1">
+      <c r="A27" s="13" t="s">
+        <v>165</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C27" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D27" s="13">
+        <v>401.0</v>
+      </c>
+    </row>
+    <row r="28" ht="15.75" customHeight="1">
+      <c r="A28" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="B28" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C28" s="13" t="s">
+        <v>167</v>
+      </c>
+      <c r="D28" s="13">
+        <v>404.0</v>
+      </c>
+    </row>
+    <row r="29" ht="15.75" customHeight="1">
+      <c r="A29" s="13" t="s">
+        <v>168</v>
+      </c>
+      <c r="B29" s="13" t="s">
+        <v>169</v>
+      </c>
+      <c r="C29" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D29" s="13">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="30" ht="15.75" customHeight="1">
+      <c r="A30" s="13" t="s">
+        <v>170</v>
+      </c>
+      <c r="B30" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D30" s="13">
+        <v>200.0</v>
+      </c>
+    </row>
+    <row r="31" ht="15.75" customHeight="1">
+      <c r="A31" s="13" t="s">
+        <v>172</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>173</v>
+      </c>
+      <c r="C31" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="13">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="32" ht="15.75" customHeight="1">
+      <c r="A32" s="13" t="s">
+        <v>174</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C32" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D32" s="13">
+        <v>400.0</v>
+      </c>
+    </row>
+    <row r="33" ht="15.75" customHeight="1">
+      <c r="A33" s="13" t="s">
+        <v>175</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="13" t="s">
+        <v>163</v>
+      </c>
+      <c r="D33" s="13">
+        <v>200.0</v>
+      </c>
+    </row>
     <row r="34" ht="15.75" customHeight="1"/>
     <row r="35" ht="15.75" customHeight="1"/>
     <row r="36" ht="15.75" customHeight="1"/>
@@ -7568,707 +7804,719 @@
         <v>2</v>
       </c>
       <c r="D1" s="13" t="s">
-        <v>159</v>
+        <v>176</v>
       </c>
       <c r="F1" s="19"/>
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>160</v>
+        <v>177</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>161</v>
+        <v>178</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F2" s="20"/>
       <c r="G2" s="21"/>
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F3" s="20"/>
       <c r="G3" s="21"/>
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F4" s="20"/>
       <c r="G4" s="21"/>
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="B5" s="13" t="s">
-        <v>168</v>
+        <v>185</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F5" s="20"/>
       <c r="G5" s="21"/>
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>169</v>
+        <v>186</v>
       </c>
       <c r="B6" s="13" t="s">
-        <v>170</v>
+        <v>187</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F6" s="20"/>
       <c r="G6" s="21"/>
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="22" t="s">
-        <v>171</v>
+        <v>188</v>
       </c>
       <c r="B7" s="13" t="s">
-        <v>172</v>
+        <v>189</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F7" s="20"/>
       <c r="G7" s="21"/>
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="22" t="s">
-        <v>173</v>
+        <v>190</v>
       </c>
       <c r="B8" s="13" t="s">
-        <v>174</v>
+        <v>191</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F8" s="20"/>
       <c r="G8" s="21"/>
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="22" t="s">
-        <v>175</v>
+        <v>192</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>176</v>
+        <v>193</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F9" s="20"/>
       <c r="G9" s="21"/>
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="22" t="s">
-        <v>177</v>
+        <v>194</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>178</v>
+        <v>195</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F10" s="20"/>
       <c r="G10" s="21"/>
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>197</v>
+      </c>
+      <c r="C11" s="13" t="s">
         <v>179</v>
-      </c>
-      <c r="B11" s="13" t="s">
-        <v>180</v>
-      </c>
-      <c r="C11" s="13" t="s">
-        <v>162</v>
       </c>
       <c r="F11" s="20"/>
       <c r="G11" s="21"/>
     </row>
     <row r="12" ht="15.75" customHeight="1">
       <c r="A12" s="22" t="s">
-        <v>181</v>
+        <v>198</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>182</v>
+        <v>199</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F12" s="20"/>
       <c r="G12" s="21"/>
     </row>
     <row r="13" ht="15.75" customHeight="1">
       <c r="A13" s="22" t="s">
-        <v>183</v>
+        <v>200</v>
       </c>
       <c r="B13" s="13" t="s">
-        <v>184</v>
+        <v>201</v>
       </c>
       <c r="C13" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F13" s="20"/>
       <c r="G13" s="21"/>
     </row>
     <row r="14" ht="15.75" customHeight="1">
       <c r="A14" s="22" t="s">
-        <v>185</v>
+        <v>202</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>186</v>
+        <v>203</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F14" s="20"/>
       <c r="G14" s="21"/>
     </row>
     <row r="15" ht="15.75" customHeight="1">
       <c r="A15" s="22" t="s">
-        <v>187</v>
+        <v>204</v>
       </c>
       <c r="B15" s="13" t="s">
-        <v>188</v>
+        <v>205</v>
       </c>
       <c r="C15" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F15" s="20"/>
       <c r="G15" s="21"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
       <c r="A16" s="22" t="s">
-        <v>189</v>
+        <v>206</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>190</v>
+        <v>207</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F16" s="20"/>
       <c r="G16" s="21"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
       <c r="A17" s="22" t="s">
-        <v>191</v>
+        <v>208</v>
       </c>
       <c r="B17" s="13" t="s">
-        <v>192</v>
+        <v>209</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F17" s="20"/>
       <c r="G17" s="21"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
       <c r="A18" s="22" t="s">
-        <v>193</v>
+        <v>210</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>194</v>
+        <v>211</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F18" s="20"/>
       <c r="G18" s="21"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
       <c r="A19" s="22" t="s">
-        <v>195</v>
+        <v>212</v>
       </c>
       <c r="B19" s="13" t="s">
-        <v>196</v>
+        <v>213</v>
       </c>
       <c r="C19" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F19" s="20"/>
       <c r="G19" s="21"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
       <c r="A20" s="22" t="s">
-        <v>197</v>
+        <v>214</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>198</v>
+        <v>215</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F20" s="20"/>
       <c r="G20" s="21"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
       <c r="A21" s="22" t="s">
-        <v>199</v>
+        <v>216</v>
       </c>
       <c r="B21" s="13" t="s">
-        <v>200</v>
+        <v>217</v>
       </c>
       <c r="C21" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F21" s="20"/>
       <c r="G21" s="21"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
       <c r="A22" s="13" t="s">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F22" s="20"/>
       <c r="G22" s="21"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
       <c r="A23" s="13" t="s">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="B23" s="13" t="s">
-        <v>204</v>
+        <v>221</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F23" s="20"/>
       <c r="G23" s="21"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
       <c r="A24" s="22" t="s">
-        <v>205</v>
+        <v>222</v>
       </c>
       <c r="B24" s="13" t="s">
-        <v>206</v>
+        <v>223</v>
       </c>
       <c r="C24" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D24" s="13" t="s">
-        <v>207</v>
+        <v>224</v>
       </c>
       <c r="F24" s="20"/>
       <c r="G24" s="21"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
       <c r="A25" s="22" t="s">
-        <v>208</v>
+        <v>225</v>
       </c>
       <c r="B25" s="13" t="s">
-        <v>209</v>
+        <v>226</v>
       </c>
       <c r="C25" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>210</v>
+        <v>227</v>
       </c>
       <c r="F25" s="20"/>
       <c r="G25" s="21"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
       <c r="A26" s="22" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>212</v>
+        <v>229</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>213</v>
+        <v>230</v>
       </c>
       <c r="F26" s="20"/>
       <c r="G26" s="21"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
       <c r="A27" s="22" t="s">
-        <v>214</v>
+        <v>231</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>215</v>
+        <v>232</v>
       </c>
       <c r="C27" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D27" s="13" t="s">
-        <v>216</v>
+        <v>233</v>
       </c>
       <c r="F27" s="20"/>
       <c r="G27" s="21"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
       <c r="A28" s="22" t="s">
-        <v>217</v>
+        <v>234</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>218</v>
+        <v>235</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D28" s="13" t="s">
-        <v>219</v>
+        <v>236</v>
       </c>
       <c r="F28" s="20"/>
       <c r="G28" s="21"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
       <c r="A29" s="22" t="s">
-        <v>220</v>
+        <v>237</v>
       </c>
       <c r="B29" s="13" t="s">
-        <v>221</v>
+        <v>238</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D29" s="13" t="s">
-        <v>222</v>
+        <v>239</v>
       </c>
       <c r="F29" s="20"/>
       <c r="G29" s="21"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
       <c r="A30" s="22" t="s">
-        <v>223</v>
+        <v>240</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>224</v>
+        <v>241</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>225</v>
+        <v>242</v>
       </c>
       <c r="F30" s="20"/>
       <c r="G30" s="21"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
       <c r="A31" s="22" t="s">
-        <v>226</v>
+        <v>243</v>
       </c>
       <c r="B31" s="13" t="s">
-        <v>227</v>
+        <v>244</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="D31" s="13" t="s">
-        <v>228</v>
+        <v>245</v>
       </c>
       <c r="F31" s="20"/>
       <c r="G31" s="21"/>
     </row>
     <row r="32" ht="15.75" customHeight="1">
       <c r="A32" s="22" t="s">
-        <v>229</v>
+        <v>246</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>230</v>
+        <v>247</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F32" s="20"/>
       <c r="G32" s="21"/>
     </row>
     <row r="33" ht="15.75" customHeight="1">
       <c r="A33" s="22" t="s">
-        <v>231</v>
+        <v>248</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>232</v>
+        <v>249</v>
       </c>
       <c r="C33" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F33" s="20"/>
       <c r="G33" s="21"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
       <c r="A34" s="22" t="s">
-        <v>233</v>
+        <v>250</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>234</v>
+        <v>251</v>
       </c>
       <c r="C34" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F34" s="20"/>
       <c r="G34" s="21"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
       <c r="A35" s="22" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>236</v>
+        <v>253</v>
       </c>
       <c r="C35" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F35" s="20"/>
       <c r="G35" s="21"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
       <c r="A36" s="22" t="s">
-        <v>237</v>
+        <v>254</v>
       </c>
       <c r="B36" s="13" t="s">
-        <v>238</v>
+        <v>255</v>
       </c>
       <c r="C36" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F36" s="20"/>
       <c r="G36" s="21"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="22" t="s">
-        <v>239</v>
+        <v>256</v>
       </c>
       <c r="B37" s="13" t="s">
-        <v>240</v>
+        <v>257</v>
       </c>
       <c r="C37" s="13" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="F37" s="20"/>
       <c r="G37" s="21"/>
     </row>
     <row r="38" ht="15.75" customHeight="1">
       <c r="A38" s="22" t="s">
-        <v>241</v>
+        <v>258</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="13" t="s">
-        <v>242</v>
+        <v>259</v>
       </c>
       <c r="F38" s="20"/>
       <c r="G38" s="21"/>
     </row>
     <row r="39" ht="15.75" customHeight="1">
       <c r="A39" s="22" t="s">
-        <v>243</v>
+        <v>260</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="13" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="F39" s="20"/>
       <c r="G39" s="21"/>
     </row>
     <row r="40" ht="15.75" customHeight="1">
       <c r="A40" s="22" t="s">
-        <v>245</v>
+        <v>262</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="13" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="F40" s="20"/>
       <c r="G40" s="21"/>
     </row>
     <row r="41" ht="15.75" customHeight="1">
       <c r="A41" s="22" t="s">
-        <v>247</v>
+        <v>264</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="13" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="F41" s="20"/>
       <c r="G41" s="21"/>
     </row>
     <row r="42" ht="15.75" customHeight="1">
       <c r="A42" s="22" t="s">
-        <v>249</v>
+        <v>266</v>
       </c>
       <c r="B42" s="13"/>
       <c r="C42" s="13" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="F42" s="20"/>
       <c r="G42" s="21"/>
     </row>
     <row r="43" ht="15.75" customHeight="1">
       <c r="A43" s="22" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="B43" s="13"/>
       <c r="C43" s="13" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="F43" s="20"/>
       <c r="G43" s="21"/>
     </row>
     <row r="44" ht="15.75" customHeight="1">
       <c r="A44" s="22" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="B44" s="13"/>
       <c r="C44" s="13" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="F44" s="20"/>
       <c r="G44" s="21"/>
     </row>
     <row r="45" ht="15.75" customHeight="1">
       <c r="A45" s="22" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="B45" s="13"/>
       <c r="C45" s="13" t="s">
-        <v>254</v>
+        <v>271</v>
       </c>
       <c r="F45" s="20"/>
       <c r="G45" s="21"/>
     </row>
     <row r="46" ht="15.75" customHeight="1">
       <c r="A46" s="22" t="s">
-        <v>255</v>
+        <v>272</v>
       </c>
       <c r="B46" s="13"/>
       <c r="C46" s="13" t="s">
-        <v>256</v>
+        <v>273</v>
       </c>
       <c r="F46" s="20"/>
       <c r="G46" s="21"/>
     </row>
     <row r="47" ht="15.75" customHeight="1">
       <c r="A47" s="22" t="s">
-        <v>257</v>
+        <v>274</v>
       </c>
       <c r="B47" s="13"/>
       <c r="C47" s="13" t="s">
-        <v>258</v>
+        <v>275</v>
       </c>
       <c r="F47" s="20"/>
       <c r="G47" s="21"/>
     </row>
     <row r="48" ht="15.75" customHeight="1">
       <c r="A48" s="22" t="s">
-        <v>259</v>
+        <v>276</v>
       </c>
       <c r="B48" s="13"/>
       <c r="C48" s="13" t="s">
-        <v>260</v>
+        <v>277</v>
       </c>
       <c r="F48" s="20"/>
       <c r="G48" s="21"/>
     </row>
     <row r="49" ht="15.75" customHeight="1">
       <c r="A49" s="22" t="s">
-        <v>261</v>
+        <v>278</v>
       </c>
       <c r="B49" s="13"/>
       <c r="C49" s="13" t="s">
-        <v>262</v>
+        <v>279</v>
       </c>
       <c r="F49" s="20"/>
       <c r="G49" s="21"/>
     </row>
     <row r="50" ht="15.75" customHeight="1">
       <c r="A50" s="22" t="s">
-        <v>263</v>
+        <v>280</v>
       </c>
       <c r="B50" s="13"/>
       <c r="C50" s="13" t="s">
-        <v>264</v>
+        <v>281</v>
       </c>
       <c r="F50" s="20"/>
       <c r="G50" s="21"/>
     </row>
     <row r="51" ht="15.75" customHeight="1">
       <c r="A51" s="22" t="s">
-        <v>265</v>
+        <v>282</v>
       </c>
       <c r="B51" s="13"/>
       <c r="C51" s="13" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="F51" s="20"/>
       <c r="G51" s="21"/>
     </row>
     <row r="52" ht="15.75" customHeight="1">
       <c r="A52" s="23" t="s">
-        <v>267</v>
+        <v>284</v>
       </c>
       <c r="B52" s="13"/>
       <c r="C52" s="13" t="s">
-        <v>268</v>
+        <v>285</v>
       </c>
       <c r="F52" s="20"/>
       <c r="G52" s="21"/>
     </row>
     <row r="53" ht="15.75" customHeight="1">
       <c r="A53" s="23" t="s">
-        <v>269</v>
+        <v>286</v>
       </c>
       <c r="B53" s="13"/>
       <c r="C53" s="13" t="s">
-        <v>270</v>
+        <v>287</v>
       </c>
       <c r="F53" s="20"/>
       <c r="G53" s="21"/>
     </row>
     <row r="54" ht="15.75" customHeight="1">
       <c r="A54" s="24" t="s">
-        <v>271</v>
+        <v>288</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="13" t="s">
-        <v>272</v>
+        <v>289</v>
       </c>
       <c r="F54" s="20"/>
       <c r="G54" s="21"/>
     </row>
     <row r="55" ht="15.75" customHeight="1">
-      <c r="A55" s="25"/>
+      <c r="A55" s="24" t="s">
+        <v>290</v>
+      </c>
       <c r="B55" s="13"/>
-      <c r="C55" s="13"/>
+      <c r="C55" s="13" t="s">
+        <v>291</v>
+      </c>
       <c r="F55" s="20"/>
       <c r="G55" s="21"/>
     </row>
     <row r="56" ht="15.75" customHeight="1">
-      <c r="A56" s="25"/>
+      <c r="A56" s="25" t="s">
+        <v>292</v>
+      </c>
       <c r="B56" s="13"/>
-      <c r="C56" s="13"/>
+      <c r="C56" s="13" t="s">
+        <v>293</v>
+      </c>
       <c r="F56" s="20"/>
       <c r="G56" s="21"/>
     </row>
     <row r="57" ht="15.75" customHeight="1">
-      <c r="A57" s="25"/>
+      <c r="A57" s="25" t="s">
+        <v>294</v>
+      </c>
       <c r="B57" s="13"/>
-      <c r="C57" s="13"/>
+      <c r="C57" s="13" t="s">
+        <v>295</v>
+      </c>
       <c r="F57" s="20"/>
       <c r="G57" s="21"/>
     </row>
@@ -8288,51 +8536,51 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="13" t="s">
-        <v>273</v>
+        <v>296</v>
       </c>
       <c r="B60" s="13"/>
       <c r="C60" s="13" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="F60" s="20"/>
       <c r="G60" s="21"/>
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="13" t="s">
-        <v>275</v>
+        <v>298</v>
       </c>
       <c r="C61" s="13" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="F61" s="20"/>
       <c r="G61" s="21"/>
     </row>
     <row r="62" ht="15.75" customHeight="1">
       <c r="A62" s="13" t="s">
-        <v>276</v>
+        <v>299</v>
       </c>
       <c r="C62" s="13" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="F62" s="20"/>
       <c r="G62" s="21"/>
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="13" t="s">
-        <v>277</v>
+        <v>300</v>
       </c>
       <c r="C63" s="13" t="s">
-        <v>274</v>
+        <v>297</v>
       </c>
       <c r="F63" s="20"/>
       <c r="G63" s="21"/>
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="13" t="s">
-        <v>278</v>
+        <v>301</v>
       </c>
       <c r="C64" s="13" t="s">
-        <v>279</v>
+        <v>302</v>
       </c>
       <c r="F64" s="20"/>
       <c r="G64" s="21"/>
@@ -8374,58 +8622,58 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="13" t="s">
-        <v>280</v>
+        <v>303</v>
       </c>
       <c r="F74" s="20"/>
       <c r="G74" s="21"/>
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="13" t="s">
-        <v>281</v>
+        <v>304</v>
       </c>
       <c r="G75" s="21"/>
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="13" t="s">
-        <v>282</v>
+        <v>305</v>
       </c>
       <c r="G76" s="21"/>
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="13" t="s">
-        <v>283</v>
+        <v>306</v>
       </c>
       <c r="F77" s="26"/>
       <c r="G77" s="21"/>
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="13" t="s">
-        <v>284</v>
+        <v>307</v>
       </c>
       <c r="G78" s="21"/>
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="13" t="s">
-        <v>285</v>
+        <v>308</v>
       </c>
       <c r="G79" s="21"/>
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="13" t="s">
-        <v>286</v>
+        <v>309</v>
       </c>
       <c r="F80" s="20"/>
       <c r="G80" s="21"/>
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="13" t="s">
-        <v>287</v>
+        <v>310</v>
       </c>
       <c r="G81" s="21"/>
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="13" t="s">
-        <v>288</v>
+        <v>311</v>
       </c>
       <c r="G82" s="21"/>
     </row>
@@ -11379,12 +11627,12 @@
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="F64:F66"/>
     <mergeCell ref="F70:F71"/>
     <mergeCell ref="F74:F76"/>
     <mergeCell ref="F77:F79"/>
     <mergeCell ref="F80:F82"/>
     <mergeCell ref="F83:F84"/>
-    <mergeCell ref="F64:F66"/>
   </mergeCells>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -11424,13 +11672,13 @@
     </row>
     <row r="2" ht="15.75" customHeight="1">
       <c r="A2" s="13" t="s">
-        <v>289</v>
+        <v>312</v>
       </c>
       <c r="B2" s="28" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D2" s="13">
         <v>201.0</v>
@@ -11438,13 +11686,13 @@
     </row>
     <row r="3" ht="15.75" customHeight="1">
       <c r="A3" s="13" t="s">
-        <v>292</v>
+        <v>315</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>290</v>
+        <v>313</v>
       </c>
       <c r="C3" s="13" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D3" s="13">
         <v>400.0</v>
@@ -11453,13 +11701,13 @@
     </row>
     <row r="4" ht="15.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>293</v>
+        <v>316</v>
       </c>
       <c r="B4" s="13" t="s">
-        <v>294</v>
+        <v>317</v>
       </c>
       <c r="C4" s="13" t="s">
-        <v>291</v>
+        <v>314</v>
       </c>
       <c r="D4" s="13">
         <v>500.0</v>
@@ -11468,10 +11716,10 @@
     </row>
     <row r="5" ht="15.75" customHeight="1">
       <c r="A5" s="13" t="s">
-        <v>295</v>
+        <v>318</v>
       </c>
       <c r="C5" s="13" t="s">
-        <v>296</v>
+        <v>319</v>
       </c>
       <c r="D5" s="13">
         <v>200.0</v>
@@ -11480,10 +11728,10 @@
     </row>
     <row r="6" ht="15.75" customHeight="1">
       <c r="A6" s="13" t="s">
-        <v>297</v>
+        <v>320</v>
       </c>
       <c r="C6" s="13" t="s">
-        <v>298</v>
+        <v>321</v>
       </c>
       <c r="D6" s="13">
         <v>200.0</v>
@@ -11492,10 +11740,10 @@
     </row>
     <row r="7" ht="15.75" customHeight="1">
       <c r="A7" s="13" t="s">
-        <v>299</v>
+        <v>322</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>300</v>
+        <v>323</v>
       </c>
       <c r="D7" s="13">
         <v>404.0</v>
@@ -11504,13 +11752,13 @@
     </row>
     <row r="8" ht="15.75" customHeight="1">
       <c r="A8" s="13" t="s">
-        <v>301</v>
+        <v>324</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>303</v>
+        <v>326</v>
       </c>
       <c r="D8" s="13">
         <v>200.0</v>
@@ -11519,13 +11767,13 @@
     </row>
     <row r="9" ht="15.75" customHeight="1">
       <c r="A9" s="13" t="s">
-        <v>304</v>
+        <v>327</v>
       </c>
       <c r="B9" s="13" t="s">
-        <v>302</v>
+        <v>325</v>
       </c>
       <c r="C9" s="13" t="s">
-        <v>305</v>
+        <v>328</v>
       </c>
       <c r="D9" s="13">
         <v>400.0</v>
@@ -11534,10 +11782,10 @@
     </row>
     <row r="10" ht="15.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>306</v>
+        <v>329</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>307</v>
+        <v>330</v>
       </c>
       <c r="D10" s="13">
         <v>200.0</v>
@@ -11546,10 +11794,10 @@
     </row>
     <row r="11" ht="15.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>308</v>
+        <v>331</v>
       </c>
       <c r="C11" s="13" t="s">
-        <v>309</v>
+        <v>332</v>
       </c>
       <c r="D11" s="13">
         <v>404.0</v>

</xml_diff>

<commit_message>
schema validation for skill master
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -776,7 +776,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teaaapi15@gmail.co</t>
+      <t>teaaapi16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -794,7 +794,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8232323209</t>
+      <t>+1 9232323209</t>
     </r>
     <r>
       <rPr>
@@ -841,7 +841,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapi15@gmail.co</t>
+      <t>teamapi16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -884,7 +884,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapia15@gmail.co</t>
+      <t>teamapia16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -902,7 +902,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8000110009</t>
+      <t>+1 9000110009</t>
     </r>
     <r>
       <rPr>
@@ -947,7 +947,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiab15@gmail.co</t>
+      <t>teamapiab16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -965,7 +965,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8000111009</t>
+      <t>+1 9000111009</t>
     </r>
     <r>
       <rPr>
@@ -1010,7 +1010,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabc15@gmail.co</t>
+      <t>teamapiabc16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1028,7 +1028,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8001111009</t>
+      <t>+1 9001111009</t>
     </r>
     <r>
       <rPr>
@@ -1073,7 +1073,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcd15@gmail.co</t>
+      <t>teamapiabcd16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1091,7 +1091,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8011111009</t>
+      <t>+1 9011111009</t>
     </r>
     <r>
       <rPr>
@@ -1136,7 +1136,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabce15@gmail.co</t>
+      <t>teamapiabce16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1154,7 +1154,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8111111009</t>
+      <t>+1 9111111009</t>
     </r>
     <r>
       <rPr>
@@ -1199,7 +1199,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcf15@gmail.co</t>
+      <t>teamapiabcf16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1217,7 +1217,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8211111009</t>
+      <t>+1 9211111009</t>
     </r>
     <r>
       <rPr>
@@ -1262,7 +1262,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcg15@gmail.co</t>
+      <t>teamapiabcg16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1280,7 +1280,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8221111009</t>
+      <t>+1 9221111009</t>
     </r>
     <r>
       <rPr>
@@ -1325,7 +1325,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabch15@gmail.co</t>
+      <t>teamapiabch16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1343,7 +1343,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8222111009</t>
+      <t>+1 9222111009</t>
     </r>
     <r>
       <rPr>
@@ -1388,7 +1388,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabci15@gmail.co</t>
+      <t>teamapiabci16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1406,7 +1406,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8222211009</t>
+      <t>+1 9222211009</t>
     </r>
     <r>
       <rPr>
@@ -1451,7 +1451,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcj15@gmail.co</t>
+      <t>teamapiabcj16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1469,7 +1469,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8222221009</t>
+      <t>+1 9222221009</t>
     </r>
     <r>
       <rPr>
@@ -1514,7 +1514,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabck15@gmail.co</t>
+      <t>teamapiabck16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1532,7 +1532,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8222222009</t>
+      <t>+1 9222222009</t>
     </r>
     <r>
       <rPr>
@@ -1577,7 +1577,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcl15@gmail.co</t>
+      <t>teamapiabcl16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1595,7 +1595,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8222222209</t>
+      <t>+1 9222222209</t>
     </r>
     <r>
       <rPr>
@@ -1640,7 +1640,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcm15@gmail.co</t>
+      <t>teamapiabcm16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1658,7 +1658,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8322222209</t>
+      <t>+1 9322222209</t>
     </r>
     <r>
       <rPr>
@@ -1703,7 +1703,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcn15@gmail.co</t>
+      <t>teamapiabcn16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1721,7 +1721,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8332222209</t>
+      <t>+1 9332222209</t>
     </r>
     <r>
       <rPr>
@@ -1766,7 +1766,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabco15@gmail.co</t>
+      <t>teamapiabco16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1784,7 +1784,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8333222209</t>
+      <t>+1 9333222209</t>
     </r>
     <r>
       <rPr>
@@ -1829,7 +1829,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcp15@gmail.co</t>
+      <t>teamapiabcp16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1847,7 +1847,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8333322209</t>
+      <t>+1 9333322209</t>
     </r>
     <r>
       <rPr>
@@ -1892,7 +1892,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcq15@gmail.co</t>
+      <t>teamapiabcq16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1910,7 +1910,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8333332209</t>
+      <t>+1 9333332209</t>
     </r>
     <r>
       <rPr>
@@ -1955,7 +1955,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcr15@gmail.co</t>
+      <t>teamapiabcr16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1973,7 +1973,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8433332209</t>
+      <t>+1 9433332209</t>
     </r>
     <r>
       <rPr>
@@ -2018,7 +2018,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcs15@gmail.co</t>
+      <t>teamapiabcs16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2029,7 +2029,7 @@
     "loginStatus": "Active",
     "status": "Active"
   },
-  "userPhoneNumber": "+1 8762345345",
+  "userPhoneNumber": "+1 9762345345",
   "userRoleMaps": [
     {
       "roleId": "R01",
@@ -2071,7 +2071,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2119,7 +2119,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2170,7 +2170,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2221,7 +2221,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2273,7 +2273,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2324,7 +2324,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2375,7 +2375,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2426,7 +2426,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2472,7 +2472,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8443332209</t>
+      <t>+1 9443332209</t>
     </r>
     <r>
       <rPr>
@@ -2520,7 +2520,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabct15@gmail.co</t>
+      <t>teamapiabct16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2538,7 +2538,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8444332209</t>
+      <t>+1 9444332209</t>
     </r>
     <r>
       <rPr>
@@ -2582,7 +2582,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcu15@gmail.co</t>
+      <t>teamapiabcu16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2600,7 +2600,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8444432209</t>
+      <t>+1 9444432209</t>
     </r>
     <r>
       <rPr>
@@ -2644,7 +2644,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcv15@gmail.co</t>
+      <t>teamapiabcv16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2662,7 +2662,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8544332209</t>
+      <t>+1 9544332209</t>
     </r>
     <r>
       <rPr>
@@ -2706,7 +2706,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcw15@gmail.co</t>
+      <t>teamapiabcw16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2724,7 +2724,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8554332209</t>
+      <t>+1 9554332209</t>
     </r>
     <r>
       <rPr>
@@ -2768,7 +2768,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcx15@gmail.co</t>
+      <t>teamapiabcx16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2786,7 +2786,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+1 8555332209</t>
+      <t>+1 9555332209</t>
     </r>
     <r>
       <rPr>
@@ -2830,7 +2830,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcy15@gmail.co</t>
+      <t>teamapiabcy16@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3024,7 +3024,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_playwrightAPI"
+"skillName": "Team1_playwrightUI"
 }</t>
   </si>
   <si>
@@ -3063,7 +3063,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_playwrightAPIUpdated"
+"skillName": "Team1_playwrightUIUpdated"
 }</t>
   </si>
   <si>

</xml_diff>

<commit_message>
updated the folder name
</commit_message>
<xml_diff>
--- a/src/test/resources/Team1_lms_TestDataSheet.xlsx
+++ b/src/test/resources/Team1_lms_TestDataSheet.xlsx
@@ -234,7 +234,7 @@
   <si>
     <t>{
  "userLoginEmailId": "team1@gmail.com",
- "password": "ApiHackathonnew8@1"
+ "password": "ApiHackathonnew99@1"
  }</t>
   </si>
   <si>
@@ -370,8 +370,8 @@
   </si>
   <si>
     <t>{
-"programDescription": "C sharp Programming",
-"programName": "C sharp Progra-m-m--i-n-g",
+"programDescription": "Cc sharp Programming",
+"programName": "Cc sharp Progr-amm--i-n-g",
  "programStatus": "Active"
 }</t>
   </si>
@@ -393,7 +393,7 @@
   <si>
     <t>{
 "programDescription": "Java Des",
- "programName": "Prog Java",
+ "programName": "Progr- Java",
  "programStatus": "Active"
 }</t>
   </si>
@@ -462,7 +462,7 @@
     <t>CreateProgram_with_space_in_the_start and end_of_ProgramName</t>
   </si>
   <si>
-    <t>{"programDescription": "Python Programming1", "programName":    "   Progr Python thr-e-e   "   , "programStatus": "Active"}</t>
+    <t>{"programDescription": "Python Programming1", "programName":    "   Progr    r Python t-hr-e-e   "   , "programStatus": "Active"}</t>
   </si>
   <si>
     <t>CreateProgram_with_Valid_ProgramDesc_ProgramName_Active_Status</t>
@@ -470,7 +470,7 @@
   <si>
     <t>{
 "programDescription": "C sharp ProgramTwo",
- "programName": "C sharp Progra-m-T-w-elve-",
+ "programName": "Cc sharp Progr-a-m-Twelv-e-",
 "programStatus": "Active"
 }</t>
   </si>
@@ -486,7 +486,7 @@
   <si>
     <t>{
 "programDescription": "C sharp Programthre", 
-"programName": "C sharp Programth--Twe--", 
+"programName": "Cc sharp Programt-h-Tw-e--", 
 "programStatus": "Active"
 }</t>
   </si>
@@ -499,14 +499,14 @@
   <si>
     <t xml:space="preserve">{
 "programDescription": "C sharp Program-four",
-"programName": "C sharp Program-f-o--u-r", 
+"programName": "J sharp Progr-a-m-f-ou-r", 
 "programStatus": "Active"
 </t>
   </si>
   <si>
     <t>{
 "programDescription": "C sharp Programf-ive",
- "programName": "C -sharp Progra-m-f-i--ve",
+ "programName": "C -s--h-arp Program-f-i-e",
 "programStatus": "Active"
 }</t>
   </si>
@@ -638,8 +638,8 @@
   </si>
   <si>
     <t>{
-"programDescription": "Java Programming-Fiiv",
- "programName": "ProgNamehe-F-iv-e",
+"programDescription": "Java Programming-Fi-iv",
+ "programName": "ProgName-f-iv-e",
 "programStatus": "Active"
 }</t>
   </si>
@@ -661,7 +661,7 @@
   <si>
     <t>{
 "programDescription": "Java Programminug six",
- "programName": "Update Phrougram ss-i---x",
+ "programName": "Update Phrougr-am s-s--i-x",
  "programStatus": "Active"
 }</t>
   </si>
@@ -743,7 +743,7 @@
   <si>
     <t>{
 "programDescription": "Fully Valid hh",
- "programName": "UpdatedhhProgram--s-ix", 
+ "programName": "UpdatedhhProg-ra-m-s-i-x", 
 "programStatus": "Active"
 }</t>
   </si>
@@ -886,7 +886,7 @@
   </si>
   <si>
     <t>{
-"batchName": "testBatch1127",
+"batchName": "testBatch1130",
 "batchNoOfClasses": 1,
 "batchStatus": "Active",
 "programId": 13
@@ -1109,7 +1109,7 @@
     <t xml:space="preserve">{ 
 "batchDescription": "test", 
 "batchId": 0, 
-"batchName": "UpdatedBatch1125", 
+"batchName": "UpdatedBatch1128", 
 "batchNoOfClasses": 1, 
 "batchStatus": "Active", 
 "programId": "", 
@@ -1197,7 +1197,7 @@
   <si>
     <t>{ 
 "batchId": 0, 
-"batchName": "TestttttBatch117", 
+"batchName": "TestttttBatch1210", 
 "batchNoOfClasses": 1, 
 "batchStatus": "Active", 
 "programId": "", 
@@ -1289,7 +1289,7 @@
     <t xml:space="preserve">{ 
 "batchDescription": "test", 
 "batchId": 0, 
-"batchName": "TestBatchhhh111", 
+"batchName": "TestBatchhhh114", 
 "batchNoOfClasses": 1, 
 "batchStatus": "Active", 
 "programId": "70", 
@@ -1354,7 +1354,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teaaapi26@gmail.co</t>
+      <t>teaaapi29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1372,7 +1372,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1232323209</t>
+      <t>+3 4232323209</t>
     </r>
     <r>
       <rPr>
@@ -1419,7 +1419,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapi26@gmail.co</t>
+      <t>teamapi29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1462,7 +1462,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapia26@gmail.co</t>
+      <t>teamapia29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1480,7 +1480,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1000110009</t>
+      <t>+3 4000110009</t>
     </r>
     <r>
       <rPr>
@@ -1525,7 +1525,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiab26@gmail.co</t>
+      <t>teamapiab29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1543,7 +1543,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1000111009</t>
+      <t>+3 4000111009</t>
     </r>
     <r>
       <rPr>
@@ -1588,7 +1588,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabc26@gmail.co</t>
+      <t>teamapiabc29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1606,7 +1606,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1001111009</t>
+      <t>+3 4001111009</t>
     </r>
     <r>
       <rPr>
@@ -1651,7 +1651,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcd26@gmail.co</t>
+      <t>teamapiabcd29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1669,7 +1669,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1011111009</t>
+      <t>+3 4011111009</t>
     </r>
     <r>
       <rPr>
@@ -1714,7 +1714,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabce26@gmail.co</t>
+      <t>teamapiabce29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1732,7 +1732,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1111111009</t>
+      <t>+3 4111111009</t>
     </r>
     <r>
       <rPr>
@@ -1777,7 +1777,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcf26@gmail.co</t>
+      <t>teamapiabcf29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1795,7 +1795,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1211111009</t>
+      <t>+3 4211111009</t>
     </r>
     <r>
       <rPr>
@@ -1840,7 +1840,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcg26@gmail.co</t>
+      <t>teamapiabcg29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1858,7 +1858,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1221111009</t>
+      <t>+3 4221111009</t>
     </r>
     <r>
       <rPr>
@@ -1903,7 +1903,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabch26@gmail.co</t>
+      <t>teamapiabch29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1921,7 +1921,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1222111009</t>
+      <t>+3 4222111009</t>
     </r>
     <r>
       <rPr>
@@ -1966,7 +1966,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabci26@gmail.co</t>
+      <t>teamapiabci29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -1984,7 +1984,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1222211009</t>
+      <t>+3 4222211009</t>
     </r>
     <r>
       <rPr>
@@ -2029,7 +2029,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcj26@gmail.co</t>
+      <t>teamapiabcj29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2047,7 +2047,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1222221009</t>
+      <t>+3 4222221009</t>
     </r>
     <r>
       <rPr>
@@ -2092,7 +2092,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabck26@gmail.co</t>
+      <t>teamapiabck29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2110,7 +2110,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1222222009</t>
+      <t>+3 4222222009</t>
     </r>
     <r>
       <rPr>
@@ -2155,7 +2155,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcl26@gmail.co</t>
+      <t>teamapiabcl29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2173,7 +2173,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1222222209</t>
+      <t>+3 4222222209</t>
     </r>
     <r>
       <rPr>
@@ -2218,7 +2218,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcm26@gmail.co</t>
+      <t>teamapiabcm29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2236,7 +2236,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1322222209</t>
+      <t>+3 4322222209</t>
     </r>
     <r>
       <rPr>
@@ -2281,7 +2281,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcn26@gmail.co</t>
+      <t>teamapiabcn29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2299,7 +2299,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1332222209</t>
+      <t>+3 4332222209</t>
     </r>
     <r>
       <rPr>
@@ -2344,7 +2344,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabco26@gmail.co</t>
+      <t>teamapiabco29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2362,7 +2362,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1333222209</t>
+      <t>+3 4333222209</t>
     </r>
     <r>
       <rPr>
@@ -2407,7 +2407,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcp26@gmail.co</t>
+      <t>teamapiabcp29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2425,7 +2425,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1333322209</t>
+      <t>+3 4333322209</t>
     </r>
     <r>
       <rPr>
@@ -2470,7 +2470,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcq26@gmail.co</t>
+      <t>teamapiabcq29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2488,7 +2488,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1333332209</t>
+      <t>+3 4333332209</t>
     </r>
     <r>
       <rPr>
@@ -2533,7 +2533,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcr26@gmail.co</t>
+      <t>teamapiabcr29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2551,7 +2551,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1433332209</t>
+      <t>+3 4433332209</t>
     </r>
     <r>
       <rPr>
@@ -2596,7 +2596,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcs26@gmail.co</t>
+      <t>teamapiabcs29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -2649,7 +2649,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2697,7 +2697,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2748,7 +2748,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2799,7 +2799,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2851,7 +2851,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2902,7 +2902,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -2953,7 +2953,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -3004,7 +3004,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -3050,7 +3050,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1443332209</t>
+      <t>+3 4443332209</t>
     </r>
     <r>
       <rPr>
@@ -3098,7 +3098,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabct26@gmail.co</t>
+      <t>teamapiabct29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3116,7 +3116,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1444332209</t>
+      <t>+3 4444332209</t>
     </r>
     <r>
       <rPr>
@@ -3160,7 +3160,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcu26@gmail.co</t>
+      <t>teamapiabcu29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3178,7 +3178,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1444432209</t>
+      <t>+3 4444432209</t>
     </r>
     <r>
       <rPr>
@@ -3222,7 +3222,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcv26@gmail.co</t>
+      <t>teamapiabcv29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3240,7 +3240,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1544332209</t>
+      <t>+3 4544332209</t>
     </r>
     <r>
       <rPr>
@@ -3284,7 +3284,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcw26@gmail.co</t>
+      <t>teamapiabcw29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3302,7 +3302,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1554332209</t>
+      <t>+3 4554332209</t>
     </r>
     <r>
       <rPr>
@@ -3346,7 +3346,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcx26@gmail.co</t>
+      <t>teamapiabcx29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3364,7 +3364,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>+3 1555332209</t>
+      <t>+3 4555332209</t>
     </r>
     <r>
       <rPr>
@@ -3408,7 +3408,7 @@
         <rFont val="Arial"/>
         <color rgb="FFFF0000"/>
       </rPr>
-      <t>teamapiabcy26@gmail.co</t>
+      <t>teamapiabcy29@gmail.co</t>
     </r>
     <r>
       <rPr>
@@ -3557,7 +3557,7 @@
   "userFirstName": "updated",
   "userLastName": "testing",
   "userLoginEmail": "updatedtesting@gmail.com",
-  "userPhoneNumber": "+3 1811111009",
+  "userPhoneNumber": "+3 4811111009",
     "userId": "U000",
   "userMiddleName": "g",
   "userLocation": "usa",
@@ -3877,7 +3877,7 @@
   </si>
   <si>
     <t>{
-  "userLoginEmail": "teamapiabczy026@gmail.com",
+  "userLoginEmail": "teamapiabczy029@gmail.com",
   "loginStatus": "Active",
   "status": "Active"
 }</t>
@@ -3960,7 +3960,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_javaoplaytUIVI"
+"skillName": "Team1_javaobjeplaytUIVI"
 }</t>
   </si>
   <si>
@@ -3999,7 +3999,7 @@
   </si>
   <si>
     <t>{
-"skillName": "Team1_javaoplaytUIVIUpdated"
+"skillName": "Team1_javaobjeplaytUIVIUpdated"
 }</t>
   </si>
   <si>

</xml_diff>